<commit_message>
minor changes to reading in files
</commit_message>
<xml_diff>
--- a/Womens Pairwise.xlsx
+++ b/Womens Pairwise.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Zenack\Dropbox\College Hockey Models\NCAA-Hockey-Pairwise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Zenack\Dropbox\College Hockey Models\NCAA_Hockey_Pairwise\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8832"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -48,61 +48,67 @@
     <t>Ohio State</t>
   </si>
   <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Northeastern</t>
+  </si>
+  <si>
     <t>Quinnipiac</t>
   </si>
   <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Northeastern</t>
-  </si>
-  <si>
     <t>Yale</t>
   </si>
   <si>
+    <t>Clarkson</t>
+  </si>
+  <si>
     <t>Colgate</t>
   </si>
   <si>
     <t>Minnesota Duluth</t>
   </si>
   <si>
-    <t>Clarkson</t>
-  </si>
-  <si>
     <t>Harvard</t>
   </si>
   <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Princeton</t>
+  </si>
+  <si>
     <t>Providence</t>
   </si>
   <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Princeton</t>
+    <t>Penn State</t>
   </si>
   <si>
     <t>Mercyhurst</t>
   </si>
   <si>
-    <t>Penn State</t>
+    <t>Vermont</t>
   </si>
   <si>
     <t>Minnesota State</t>
   </si>
   <si>
+    <t>Bemidji State</t>
+  </si>
+  <si>
+    <t>Boston College</t>
+  </si>
+  <si>
+    <t>St. Lawrence</t>
+  </si>
+  <si>
     <t>Boston University</t>
   </si>
   <si>
-    <t>Bemidji State</t>
-  </si>
-  <si>
-    <t>Boston College</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>St. Lawrence</t>
+    <t>Cornell</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
   </si>
   <si>
     <t>LIU</t>
@@ -111,15 +117,12 @@
     <t>Maine</t>
   </si>
   <si>
-    <t>Cornell</t>
+    <t>New Hampshire</t>
   </si>
   <si>
     <t>St. Cloud State</t>
   </si>
   <si>
-    <t>Syracuse</t>
-  </si>
-  <si>
     <t>Rensselaer</t>
   </si>
   <si>
@@ -130,9 +133,6 @@
   </si>
   <si>
     <t>St. Anselm</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
   </si>
   <si>
     <t>St. Thomas</t>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,16 +550,16 @@
         <v>40</v>
       </c>
       <c r="D2">
-        <v>0.67423170439729696</v>
+        <v>0.66524448105191614</v>
       </c>
       <c r="E2">
-        <v>9.285714285714286E-3</v>
+        <v>9.5454545454545462E-3</v>
       </c>
       <c r="F2">
-        <v>0.66494599011158273</v>
+        <v>0.65569902650646161</v>
       </c>
       <c r="G2">
-        <v>0.64331701932601371</v>
+        <v>0.63980469472921186</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -573,16 +573,16 @@
         <v>39</v>
       </c>
       <c r="D3">
-        <v>0.65314181349457401</v>
+        <v>0.65108080672620039</v>
       </c>
       <c r="E3">
-        <v>6.666666666666668E-3</v>
+        <v>7.000000000000001E-3</v>
       </c>
       <c r="F3">
-        <v>0.6464751468279073</v>
+        <v>0.64408080672620038</v>
       </c>
       <c r="G3">
-        <v>0.63788114160978382</v>
+        <v>0.63156992653084698</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -596,16 +596,16 @@
         <v>38</v>
       </c>
       <c r="D4">
-        <v>0.64196462357510797</v>
+        <v>0.63657578126705161</v>
       </c>
       <c r="E4">
-        <v>5.4385964912280734E-3</v>
+        <v>8.4848484848484857E-3</v>
       </c>
       <c r="F4">
-        <v>0.63652602708387995</v>
+        <v>0.62809093278220307</v>
       </c>
       <c r="G4">
-        <v>0.62950665938395023</v>
+        <v>0.61654115355530292</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -619,16 +619,16 @@
         <v>37</v>
       </c>
       <c r="D5">
-        <v>0.64039216375771224</v>
+        <v>0.62888458629639488</v>
       </c>
       <c r="E5">
-        <v>9.8333333333333363E-3</v>
+        <v>9.5238095238095357E-4</v>
       </c>
       <c r="F5">
-        <v>0.63055883042437888</v>
+        <v>0.62793220534401395</v>
       </c>
       <c r="G5">
-        <v>0.62018642145383096</v>
+        <v>0.62342054724956608</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -642,16 +642,16 @@
         <v>36</v>
       </c>
       <c r="D6">
-        <v>0.63482178223503749</v>
+        <v>0.62248149721613255</v>
       </c>
       <c r="E6">
-        <v>9.2105263157894854E-4</v>
+        <v>6.1111111111111132E-3</v>
       </c>
       <c r="F6">
-        <v>0.63390072960345856</v>
+        <v>0.61637038610502148</v>
       </c>
       <c r="G6">
-        <v>0.62738085297801249</v>
+        <v>0.61224954037436152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -665,16 +665,16 @@
         <v>35</v>
       </c>
       <c r="D7">
-        <v>0.61106697342913818</v>
+        <v>0.61109238814711953</v>
       </c>
       <c r="E7">
-        <v>6.1904761904761924E-3</v>
+        <v>5.9523809523809538E-3</v>
       </c>
       <c r="F7">
-        <v>0.60487649723866199</v>
+        <v>0.60514000719473859</v>
       </c>
       <c r="G7">
-        <v>0.60487649723866199</v>
+        <v>0.60514000719473859</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -688,16 +688,16 @@
         <v>34</v>
       </c>
       <c r="D8">
-        <v>0.59792505821374187</v>
+        <v>0.60738346246647912</v>
       </c>
       <c r="E8">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F8">
-        <v>0.59542505821374192</v>
+        <v>0.60488346246647917</v>
       </c>
       <c r="G8">
-        <v>0.5864707155460428</v>
+        <v>0.60140754329699864</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -711,16 +711,16 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>0.59267712178625498</v>
+        <v>0.59998261494397342</v>
       </c>
       <c r="E9">
-        <v>9.5370370370370383E-3</v>
+        <v>2.9761904761904769E-3</v>
       </c>
       <c r="F9">
-        <v>0.58314008474921797</v>
+        <v>0.59700642446778296</v>
       </c>
       <c r="G9">
-        <v>0.58314008474921797</v>
+        <v>0.58815076160143676</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -734,16 +734,16 @@
         <v>32</v>
       </c>
       <c r="D10">
-        <v>0.59070959601521622</v>
+        <v>0.59054115778911742</v>
       </c>
       <c r="E10">
-        <v>5.0000000000000023E-4</v>
+        <v>1.046296296296296E-2</v>
       </c>
       <c r="F10">
-        <v>0.59020959601521628</v>
+        <v>0.58007819482615441</v>
       </c>
       <c r="G10">
-        <v>0.58815735457917317</v>
+        <v>0.58007819482615441</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -757,16 +757,16 @@
         <v>31</v>
       </c>
       <c r="D11">
-        <v>0.56502560627490916</v>
+        <v>0.56611508784925602</v>
       </c>
       <c r="E11">
         <v>1.3095238095238099E-3</v>
       </c>
       <c r="F11">
-        <v>0.5637160824653854</v>
+        <v>0.56480556403973226</v>
       </c>
       <c r="G11">
-        <v>0.5637160824653854</v>
+        <v>0.56480556403973226</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -780,16 +780,16 @@
         <v>30</v>
       </c>
       <c r="D12">
-        <v>0.56316655082705858</v>
+        <v>0.55377026098077242</v>
       </c>
       <c r="E12">
-        <v>6.805555555555556E-3</v>
+        <v>1.1827660063478229E-19</v>
       </c>
       <c r="F12">
-        <v>0.55636099527150307</v>
+        <v>0.55377026098077242</v>
       </c>
       <c r="G12">
-        <v>0.55636099527150307</v>
+        <v>0.55117465562440282</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -803,16 +803,16 @@
         <v>29</v>
       </c>
       <c r="D13">
-        <v>0.56057817771873075</v>
+        <v>0.54502016196212932</v>
       </c>
       <c r="E13">
-        <v>1.2500000000000011E-4</v>
+        <v>5.4687500000000014E-3</v>
       </c>
       <c r="F13">
-        <v>0.56045317771873071</v>
+        <v>0.5395514119621293</v>
       </c>
       <c r="G13">
-        <v>0.55709133401874755</v>
+        <v>0.5395514119621293</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -823,19 +823,19 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>0.5543164070619151</v>
+        <v>0.53462849940611057</v>
       </c>
       <c r="E14">
-        <v>7.3214285714285733E-3</v>
+        <v>6.000000000000001E-3</v>
       </c>
       <c r="F14">
-        <v>0.54699497849048651</v>
+        <v>0.52862849940611056</v>
       </c>
       <c r="G14">
-        <v>0.54699497849048651</v>
+        <v>0.52862849940611056</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -849,16 +849,16 @@
         <v>27</v>
       </c>
       <c r="D15">
-        <v>0.52224751760283927</v>
+        <v>0.5252594901171449</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F15">
-        <v>0.52224751760283927</v>
+        <v>0.5242594901171449</v>
       </c>
       <c r="G15">
-        <v>0.52224751760283927</v>
+        <v>0.5242594901171449</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -872,16 +872,16 @@
         <v>26</v>
       </c>
       <c r="D16">
-        <v>0.51510670488784116</v>
+        <v>0.52033293339841613</v>
       </c>
       <c r="E16">
-        <v>1.052631578947369E-3</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0.51405407330889374</v>
+        <v>0.52033293339841613</v>
       </c>
       <c r="G16">
-        <v>0.51405407330889374</v>
+        <v>0.52033293339841613</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -895,16 +895,16 @@
         <v>25</v>
       </c>
       <c r="D17">
-        <v>0.51474548404830123</v>
+        <v>0.51634466268263468</v>
       </c>
       <c r="E17">
-        <v>1E-3</v>
+        <v>6.0606060606060639E-4</v>
       </c>
       <c r="F17">
-        <v>0.51374548404830123</v>
+        <v>0.51573860207657407</v>
       </c>
       <c r="G17">
-        <v>0.51374548404830123</v>
+        <v>0.51573860207657407</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="D18">
-        <v>0.51242602104025148</v>
+        <v>0.51267806604548605</v>
       </c>
       <c r="E18">
-        <v>2.631578947368421E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F18">
-        <v>0.50979444209288305</v>
+        <v>0.51167806604548605</v>
       </c>
       <c r="G18">
-        <v>0.50979444209288305</v>
+        <v>0.51167806604548605</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -941,16 +941,16 @@
         <v>23</v>
       </c>
       <c r="D19">
-        <v>0.51223547981701734</v>
+        <v>0.51130591975094819</v>
       </c>
       <c r="E19">
-        <v>3.375E-3</v>
+        <v>3.7500000000000012E-3</v>
       </c>
       <c r="F19">
-        <v>0.50886047981701732</v>
+        <v>0.50755591975094816</v>
       </c>
       <c r="G19">
-        <v>0.50886047981701732</v>
+        <v>0.50755591975094816</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -964,16 +964,16 @@
         <v>22</v>
       </c>
       <c r="D20">
-        <v>0.50873400282467174</v>
+        <v>0.50714484393786374</v>
       </c>
       <c r="E20">
-        <v>1.8518518518518539E-4</v>
+        <v>1.9274705288631189E-19</v>
       </c>
       <c r="F20">
-        <v>0.50854881763948656</v>
+        <v>0.50714484393786374</v>
       </c>
       <c r="G20">
-        <v>0.50854881763948656</v>
+        <v>0.50714484393786374</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -987,16 +987,16 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>0.50845113584946533</v>
+        <v>0.50598832218893608</v>
       </c>
       <c r="E21">
-        <v>1.7543859649122819E-4</v>
+        <v>1.9583333333333341E-3</v>
       </c>
       <c r="F21">
-        <v>0.50827569725297406</v>
+        <v>0.5040299888556028</v>
       </c>
       <c r="G21">
-        <v>0.50827569725297406</v>
+        <v>0.5040299888556028</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1007,19 +1007,19 @@
         <v>27</v>
       </c>
       <c r="C22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>0.50191825927908618</v>
+        <v>0.50397395993637395</v>
       </c>
       <c r="E22">
-        <v>1.8333333333333339E-3</v>
+        <v>2.2500000000000011E-3</v>
       </c>
       <c r="F22">
-        <v>0.50008492594575282</v>
+        <v>0.50172395993637398</v>
       </c>
       <c r="G22">
-        <v>0.50008492594575282</v>
+        <v>0.50172395993637398</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1033,16 +1033,16 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>0.48833345759702879</v>
+        <v>0.49238243748658522</v>
       </c>
       <c r="E23">
-        <v>6.1403508771929848E-4</v>
+        <v>3.8461538461538499E-4</v>
       </c>
       <c r="F23">
-        <v>0.48771942250930961</v>
+        <v>0.4919978221019698</v>
       </c>
       <c r="G23">
-        <v>0.48565743976882292</v>
+        <v>0.4919978221019698</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1056,16 +1056,16 @@
         <v>18</v>
       </c>
       <c r="D24">
-        <v>0.48426997622584389</v>
+        <v>0.489624258143253</v>
       </c>
       <c r="E24">
-        <v>1.052631578947369E-3</v>
+        <v>1.3095238095238099E-3</v>
       </c>
       <c r="F24">
-        <v>0.48321734464689647</v>
+        <v>0.48831473433372918</v>
       </c>
       <c r="G24">
-        <v>0.48321734464689647</v>
+        <v>0.48831473433372918</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1079,16 +1079,16 @@
         <v>17</v>
       </c>
       <c r="D25">
-        <v>0.48348501678514533</v>
+        <v>0.48165447499144692</v>
       </c>
       <c r="E25">
-        <v>4.3368086899420177E-19</v>
+        <v>5.3030303030303047E-4</v>
       </c>
       <c r="F25">
-        <v>0.48348501678514533</v>
+        <v>0.48112417196114382</v>
       </c>
       <c r="G25">
-        <v>0.48348501678514533</v>
+        <v>0.48007948155215552</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1102,16 +1102,16 @@
         <v>16</v>
       </c>
       <c r="D26">
-        <v>0.47773236857305829</v>
+        <v>0.47580219468251578</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>7.5000000000000067E-4</v>
       </c>
       <c r="F26">
-        <v>0.47773236857305829</v>
+        <v>0.4750521946825158</v>
       </c>
       <c r="G26">
-        <v>0.47773236857305829</v>
+        <v>0.4750521946825158</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1125,16 +1125,16 @@
         <v>15</v>
       </c>
       <c r="D27">
-        <v>0.47558734135340169</v>
+        <v>0.47138795035507991</v>
       </c>
       <c r="E27">
-        <v>1.0416666666666671E-3</v>
+        <v>4.7310640253912917E-19</v>
       </c>
       <c r="F27">
-        <v>0.47454567468673509</v>
+        <v>0.47138795035507991</v>
       </c>
       <c r="G27">
-        <v>0.47454567468673509</v>
+        <v>0.47138795035507991</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1148,16 +1148,16 @@
         <v>14</v>
       </c>
       <c r="D28">
-        <v>0.46311308270902662</v>
+        <v>0.46726249816930138</v>
       </c>
       <c r="E28">
-        <v>1.052631578947369E-3</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0.46206045113007932</v>
+        <v>0.46726249816930138</v>
       </c>
       <c r="G28">
-        <v>0.46206045113007932</v>
+        <v>0.46726249816930138</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1171,16 +1171,16 @@
         <v>13</v>
       </c>
       <c r="D29">
-        <v>0.46023813304352512</v>
+        <v>0.459843050686493</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>6.3492063492063546E-4</v>
       </c>
       <c r="F29">
-        <v>0.46023813304352512</v>
+        <v>0.45920813005157229</v>
       </c>
       <c r="G29">
-        <v>0.46023813304352512</v>
+        <v>0.45920813005157229</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1194,16 +1194,16 @@
         <v>12</v>
       </c>
       <c r="D30">
-        <v>0.45913445699082378</v>
+        <v>0.45876547932522438</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0.45913445699082378</v>
+        <v>0.45876547932522438</v>
       </c>
       <c r="G30">
-        <v>0.45913445699082378</v>
+        <v>0.45876547932522438</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1217,16 +1217,16 @@
         <v>11</v>
       </c>
       <c r="D31">
-        <v>0.45302377509174863</v>
+        <v>0.45414542743547309</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0.45302377509174863</v>
+        <v>0.45414542743547309</v>
       </c>
       <c r="G31">
-        <v>0.45302377509174863</v>
+        <v>0.45414542743547309</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1240,16 +1240,16 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <v>0.45025482468096628</v>
+        <v>0.45010644050804882</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.45025482468096628</v>
+        <v>0.45010644050804882</v>
       </c>
       <c r="G32">
-        <v>0.45025482468096628</v>
+        <v>0.45010644050804882</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1263,16 +1263,16 @@
         <v>9</v>
       </c>
       <c r="D33">
-        <v>0.4472538653408461</v>
+        <v>0.44388101031197519</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.4472538653408461</v>
+        <v>0.44388101031197519</v>
       </c>
       <c r="G33">
-        <v>0.4472538653408461</v>
+        <v>0.44388101031197519</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1286,16 +1286,16 @@
         <v>8</v>
       </c>
       <c r="D34">
-        <v>0.43870966072689221</v>
+        <v>0.4370837533891534</v>
       </c>
       <c r="E34">
-        <v>5.0000000000000023E-4</v>
+        <v>4.5454545454545482E-4</v>
       </c>
       <c r="F34">
-        <v>0.43820966072689221</v>
+        <v>0.43662920793460802</v>
       </c>
       <c r="G34">
-        <v>0.43820966072689221</v>
+        <v>0.43662920793460802</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1309,16 +1309,16 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>0.42713109242317882</v>
+        <v>0.4300829886453143</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0.42713109242317882</v>
+        <v>0.4300829886453143</v>
       </c>
       <c r="G35">
-        <v>0.42713109242317882</v>
+        <v>0.4300829886453143</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1332,16 +1332,16 @@
         <v>6</v>
       </c>
       <c r="D36">
-        <v>0.42035684043584132</v>
+        <v>0.42129102836791071</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.42035684043584132</v>
+        <v>0.42129102836791071</v>
       </c>
       <c r="G36">
-        <v>0.42035684043584132</v>
+        <v>0.42129102836791071</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1355,16 +1355,16 @@
         <v>5</v>
       </c>
       <c r="D37">
-        <v>0.4001056850341958</v>
+        <v>0.40796067000127012</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0.4001056850341958</v>
+        <v>0.40796067000127012</v>
       </c>
       <c r="G37">
-        <v>0.4001056850341958</v>
+        <v>0.40796067000127012</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1378,16 +1378,16 @@
         <v>4</v>
       </c>
       <c r="D38">
-        <v>0.39711149388377243</v>
+        <v>0.39835397651877502</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0.39711149388377243</v>
+        <v>0.39835397651877502</v>
       </c>
       <c r="G38">
-        <v>0.39711149388377243</v>
+        <v>0.39835397651877502</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1401,16 +1401,16 @@
         <v>3</v>
       </c>
       <c r="D39">
-        <v>0.39560067358582329</v>
+        <v>0.39574293546445399</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0.39560067358582329</v>
+        <v>0.39574293546445399</v>
       </c>
       <c r="G39">
-        <v>0.39560067358582329</v>
+        <v>0.39574293546445399</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1424,16 +1424,16 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>0.34724394991243301</v>
+        <v>0.35033230149466832</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.34724394991243301</v>
+        <v>0.35033230149466832</v>
       </c>
       <c r="G40">
-        <v>0.34724394991243301</v>
+        <v>0.35033230149466832</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1447,16 +1447,16 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>0.30129420070500579</v>
+        <v>0.29893326247265972</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.30129420070500579</v>
+        <v>0.29893326247265972</v>
       </c>
       <c r="G41">
-        <v>0.30129420070500579</v>
+        <v>0.29893326247265972</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1470,16 +1470,16 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>0.27672033691834641</v>
+        <v>0.27500448633831942</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0.27672033691834641</v>
+        <v>0.27500448633831942</v>
       </c>
       <c r="G42">
-        <v>0.27672033691834641</v>
+        <v>0.27500448633831942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>